<commit_message>
adding additions papers, removing birds
</commit_message>
<xml_diff>
--- a/Data/taxonomic groups.xlsx
+++ b/Data/taxonomic groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinmacartney/Documents/Protein_viability/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3673C0-2FE7-974C-A32C-8232E00883B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AC06B1-9A50-2D46-A0A8-59F8F62A46E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{180FDBA8-7599-294A-B409-3B6334D4E221}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="15">
   <si>
     <t>Calanoida</t>
   </si>
   <si>
-    <t>order</t>
-  </si>
-  <si>
     <t>Neuroptera</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Trombidiformes</t>
   </si>
   <si>
-    <t>Galliformes</t>
-  </si>
-  <si>
     <t>Araneae</t>
   </si>
   <si>
@@ -84,10 +78,7 @@
     <t>arachnid</t>
   </si>
   <si>
-    <t>bird</t>
-  </si>
-  <si>
-    <t>broad group</t>
+    <t>Orthoptera</t>
   </si>
 </sst>
 </file>
@@ -447,260 +438,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDF616-D00D-3B4A-B201-246D60BAE35E}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -708,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -716,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -724,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -732,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -740,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -748,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -756,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -764,100 +755,92 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D52">
-    <sortCondition descending="1" ref="B1:B52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D49">
+    <sortCondition descending="1" ref="B1:B49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>